<commit_message>
vvoInvoice can create an xlsx file
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -14,162 +14,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
-  <si>
-    <t>Page 3 of 7</t>
-  </si>
-  <si>
-    <t>W101</t>
-  </si>
-  <si>
-    <t>Luxottlca USA LLC</t>
-  </si>
-  <si>
-    <t>12 Harbor Park Drive</t>
-  </si>
-  <si>
-    <t>Port Washington, NY 1 1 050 Document Nomate: 8015399089 / 06/19/2017</t>
-  </si>
-  <si>
-    <t>U.S.A. Delivery Note NoJDate: 869536712 / 06/19/201 7</t>
-  </si>
-  <si>
-    <t>Order NumberlDate: 2017989667 / 06/17/2017</t>
-  </si>
-  <si>
-    <t>Customer Number: 21088782</t>
-  </si>
-  <si>
-    <t>Order Type: ZH03</t>
-  </si>
-  <si>
-    <t>Tel: 800 - 422 - 2020</t>
-  </si>
-  <si>
-    <t>Fax: 800 - 451 - 4839</t>
-  </si>
-  <si>
-    <t>MY.LUXOTTICA.COM</t>
-  </si>
-  <si>
-    <t>D-U-N-S-O1 -2697983</t>
-  </si>
-  <si>
-    <t>Bill-To Address Sold-To Address</t>
-  </si>
-  <si>
-    <t>21088782</t>
-  </si>
-  <si>
-    <t>VALLEY VISION OPTOMETRY</t>
-  </si>
-  <si>
-    <t>3028 CASTRO VALLEY BLVD 3028 CASTRO VALLEY BLVD</t>
-  </si>
-  <si>
-    <t>CASTRO VALLEY CA 94546</t>
-  </si>
-  <si>
-    <t>Terms of Payment: 2%,10/EOM</t>
-  </si>
-  <si>
-    <t>Shipping Method: UPS GROUND</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>Extended Price</t>
-  </si>
-  <si>
-    <t>Qty Unit Price Discount</t>
-  </si>
-  <si>
-    <t>Item Order Number Style Descriptlon</t>
-  </si>
-  <si>
-    <t>25 2017989667 OR 5245 ACETATE MAN OPTICAL FRAME</t>
-  </si>
-  <si>
-    <t>UPC CO R SIZE TEMPLE</t>
-  </si>
-  <si>
-    <t>805289517450 03 - TOP BLACK ON 54 145 1</t>
-  </si>
-  <si>
-    <t>Promotional Discount</t>
-  </si>
-  <si>
-    <t>ACETATE UNISEX OPTICAL FRAME</t>
-  </si>
-  <si>
-    <t>' SIZE TEMPLE</t>
-  </si>
-  <si>
-    <t>1ATTE BLACK 55 145 1</t>
-  </si>
-  <si>
-    <t>29 2017989667 ORX5268 ACETATE UNISEX OPTICAL FRAME</t>
-  </si>
-  <si>
-    <t>UPC 0 R SIZE TEMPLE</t>
-  </si>
-  <si>
-    <t>805367258598 5211 MATTE HAVANA 55 145 1</t>
-  </si>
-  <si>
-    <t>31 2017989667 CR 5 7 ACETATE MAN OPTICAL FRAME</t>
-  </si>
-  <si>
-    <t>UPC COL R SIZE TEMPLE</t>
-  </si>
-  <si>
-    <t>8053672081299 07 ~SANDBLASTED B 54 140 1 $56.00 $50.40</t>
-  </si>
-  <si>
-    <t>ACETATE MAN OPTICAL FRAME</t>
-  </si>
-  <si>
-    <t>SIZE TEMPLE</t>
-  </si>
-  <si>
-    <t>713132447178 20 O - HINY BLACK 54 140 1 $56.00</t>
-  </si>
-  <si>
-    <t>35 2017989667 0R METAL UNISEX OPTICAL FRAME</t>
-  </si>
-  <si>
-    <t>UPC 0 on SIZE TEMPLE</t>
-  </si>
-  <si>
-    <t>713132447499 250 -SH|NY BLACK 53 145 1 $68.99 $6209</t>
-  </si>
-  <si>
-    <t>Promotional Discount 101000 %</t>
-  </si>
-  <si>
-    <t>$54.52 $58 07</t>
-  </si>
-  <si>
-    <t>27 2017989667 0'</t>
-  </si>
-  <si>
-    <t>U PC</t>
-  </si>
-  <si>
-    <t>8053672585964 5</t>
-  </si>
-  <si>
-    <t>$55.59 $50.03</t>
-  </si>
-  <si>
-    <t>33 2017989667 0RX5277</t>
-  </si>
-  <si>
-    <t>10.000 90</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+  <si>
+    <t>MARCHC) N'</t>
+  </si>
+  <si>
+    <t>35 Hub Dr, Melville, New York, 11747- USA</t>
+  </si>
+  <si>
+    <t>800-645-1300 Fax: 800-544-1334</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>PAGE 1 of 1 ,</t>
+  </si>
+  <si>
+    <t>SHlP-TO Delivery 1’3</t>
+  </si>
+  <si>
+    <t>VALLEY VISION OPTOMETRY 8013974087</t>
+  </si>
+  <si>
+    <t>3028 CASTRO VALLEY BLVD INVOICE Number Date</t>
+  </si>
+  <si>
+    <t>CASTRO VALLEY CA 94546 9523941525 03/31/2017</t>
+  </si>
+  <si>
+    <t>Sold-To Code Payer Code Ship to Code</t>
+  </si>
+  <si>
+    <t>1808878 1808878 1808878</t>
+  </si>
+  <si>
+    <t>Sold-To TERMS</t>
+  </si>
+  <si>
+    <t>VALLEY VISION OPTOMETRY US 2% ‘0 Net 30 EOM</t>
+  </si>
+  <si>
+    <t>3028 CASTRO VALLEY BLVD DEPT.# DUN'S # CARTON COUNT</t>
+  </si>
+  <si>
+    <t>CASTRO VALLEY CA 94546 0</t>
+  </si>
+  <si>
+    <t>PO NUMBER SHIPMENT METHOD TYPE OF ORDER DATE OF ORDER</t>
+  </si>
+  <si>
+    <t>liao MESSENGER o5 RX Order 03/80/2017</t>
+  </si>
+  <si>
+    <t>QTY STYLE / COLOR SIZE UPC NUMBER UNIT PRICE DISCOUNT EXTENDED PRICE</t>
+  </si>
+  <si>
+    <t>/ORDER REASON /SALES ORDER</t>
+  </si>
+  <si>
+    <t>1 NIKE 7090 / MATTE NAVY/PHOTO BLUE 5317-411 78.00 0 % 78.00</t>
+  </si>
+  <si>
+    <t>INJECTED OPHTHALMIC 088689530448</t>
+  </si>
+  <si>
+    <t>RX:FEDOROWICZ 1</t>
+  </si>
+  <si>
+    <t>15873951</t>
+  </si>
+  <si>
+    <t>1 NIKE 8091 / BLACK METAL OPHTHALMIC 4817-001 73.00 0 % 73.00</t>
+  </si>
+  <si>
+    <t>RX:STOCK 088312187536</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1 NIKE 8091 / GUNMETAL/SLATE BLUE METAL 4817-923 73.00 0 % 73.00</t>
+  </si>
+  <si>
+    <t>OPHTHALMIC 088312187690</t>
+  </si>
+  <si>
+    <t>RX:STOCK 3</t>
+  </si>
+  <si>
+    <t>3 Sub Total 224.00</t>
+  </si>
+  <si>
+    <t>Postage/lns 8.81</t>
+  </si>
+  <si>
+    <t>Tax 21 .53</t>
+  </si>
+  <si>
+    <t>**** Payable in 050 **** TOTAL 254.84</t>
+  </si>
+  <si>
+    <t>STOP BY AND SEE WHAT'S NEW AT VISION EXPO</t>
+  </si>
+  <si>
+    <t>EAST</t>
   </si>
 </sst>
 </file>
@@ -501,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A63"/>
+  <dimension ref="A1:A37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -584,217 +533,112 @@
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vvoInvoice can now distinguish between different invoices
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -14,111 +14,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
-  <si>
-    <t>MARCHC) N'</t>
-  </si>
-  <si>
-    <t>35 Hub Dr, Melville, New York, 11747- USA</t>
-  </si>
-  <si>
-    <t>800-645-1300 Fax: 800-544-1334</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>PAGE 1 of 1 ,</t>
-  </si>
-  <si>
-    <t>SHlP-TO Delivery 1’3</t>
-  </si>
-  <si>
-    <t>VALLEY VISION OPTOMETRY 8013974087</t>
-  </si>
-  <si>
-    <t>3028 CASTRO VALLEY BLVD INVOICE Number Date</t>
-  </si>
-  <si>
-    <t>CASTRO VALLEY CA 94546 9523941525 03/31/2017</t>
-  </si>
-  <si>
-    <t>Sold-To Code Payer Code Ship to Code</t>
-  </si>
-  <si>
-    <t>1808878 1808878 1808878</t>
-  </si>
-  <si>
-    <t>Sold-To TERMS</t>
-  </si>
-  <si>
-    <t>VALLEY VISION OPTOMETRY US 2% ‘0 Net 30 EOM</t>
-  </si>
-  <si>
-    <t>3028 CASTRO VALLEY BLVD DEPT.# DUN'S # CARTON COUNT</t>
-  </si>
-  <si>
-    <t>CASTRO VALLEY CA 94546 0</t>
-  </si>
-  <si>
-    <t>PO NUMBER SHIPMENT METHOD TYPE OF ORDER DATE OF ORDER</t>
-  </si>
-  <si>
-    <t>liao MESSENGER o5 RX Order 03/80/2017</t>
-  </si>
-  <si>
-    <t>QTY STYLE / COLOR SIZE UPC NUMBER UNIT PRICE DISCOUNT EXTENDED PRICE</t>
-  </si>
-  <si>
-    <t>/ORDER REASON /SALES ORDER</t>
-  </si>
-  <si>
-    <t>1 NIKE 7090 / MATTE NAVY/PHOTO BLUE 5317-411 78.00 0 % 78.00</t>
-  </si>
-  <si>
-    <t>INJECTED OPHTHALMIC 088689530448</t>
-  </si>
-  <si>
-    <t>RX:FEDOROWICZ 1</t>
-  </si>
-  <si>
-    <t>15873951</t>
-  </si>
-  <si>
-    <t>1 NIKE 8091 / BLACK METAL OPHTHALMIC 4817-001 73.00 0 % 73.00</t>
-  </si>
-  <si>
-    <t>RX:STOCK 088312187536</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>1 NIKE 8091 / GUNMETAL/SLATE BLUE METAL 4817-923 73.00 0 % 73.00</t>
-  </si>
-  <si>
-    <t>OPHTHALMIC 088312187690</t>
-  </si>
-  <si>
-    <t>RX:STOCK 3</t>
-  </si>
-  <si>
-    <t>3 Sub Total 224.00</t>
-  </si>
-  <si>
-    <t>Postage/lns 8.81</t>
-  </si>
-  <si>
-    <t>Tax 21 .53</t>
-  </si>
-  <si>
-    <t>**** Payable in 050 **** TOTAL 254.84</t>
-  </si>
-  <si>
-    <t>STOP BY AND SEE WHAT'S NEW AT VISION EXPO</t>
-  </si>
-  <si>
-    <t>EAST</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+  <si>
+    <t>‘ " ' V ‘ “ “ IIIIIIlIIIIlIJIIIIIIII|||I||III|||I|||||||||||lllllllllllll|</t>
+  </si>
+  <si>
+    <t>13:00 0001</t>
+  </si>
+  <si>
+    <t>a 1 0 US 801 Jefferson Rd. _ ® For Reordering:</t>
+  </si>
+  <si>
+    <t>Par51ppany NJ 07054—3710 CALL TOLL FREE Fax</t>
+  </si>
+  <si>
+    <t>Duns# 04—681-4760 ' Nat (800) 631-1188 Nat (800) 338-5583</t>
+  </si>
+  <si>
+    <t>** WWW.MYSAFILO.COM ** NJ (800) 772—2157</t>
+  </si>
+  <si>
+    <t>ESB FILLED BACKORDER G R O U P /,</t>
+  </si>
+  <si>
+    <t>Bill TO: 1320825 Sold TC: 1320825 Ship TO: 1320825</t>
+  </si>
+  <si>
+    <t>VALLEY VISION OPTOMETRY VALLEY VISION OPTOMETRY VALLEY VISION OPTOMETRY</t>
+  </si>
+  <si>
+    <t>3028 CASTRO VALLEY BLVD 3028 CASTRO VALLEY BLVD 3028 CASTRO VALLEY BLVD</t>
+  </si>
+  <si>
+    <t>CASTRO VALLEY CA 94546 ‘ CASTRO VALLEY CA 94546 CASTRO VALLEY CA 94546</t>
+  </si>
+  <si>
+    <t>Order Ref. Trans Store Dept. Invoice Invoice</t>
+  </si>
+  <si>
+    <t>No. Order Date Code Disc Terms Customer P.O. Ship VIA Num. Num. Date Number Page</t>
+  </si>
+  <si>
+    <t>0rd P Item Description Rep # Customer List Disc Net Extended</t>
+  </si>
+  <si>
+    <t>Location t T Color/Size UPC Number Rep PO Reference Comments Price % Unit Price</t>
+  </si>
+  <si>
+    <t>MJ SML HARD/CLOTH SAF 753 N/C</t>
+  </si>
+  <si>
+    <t>800440 800440 P Pkg 0110635</t>
+  </si>
+  <si>
+    <t>1 MARC 64 BLACK |||||||||||||||||||Illlllll|| SAF 753 .</t>
+  </si>
+  <si>
+    <t>065Z 00 53/17 140 127646 Frame 827886678518 0110635</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>P‘ &lt;</t>
+  </si>
+  <si>
+    <t>Merchandise Amount:</t>
+  </si>
+  <si>
+    <t>Tax: 5.47</t>
+  </si>
+  <si>
+    <t>Shipping &amp; Insurance: FREE</t>
+  </si>
+  <si>
+    <t>Total Due: 63.07</t>
+  </si>
+  <si>
+    <t>Thank You. We appreciate your business.</t>
+  </si>
+  <si>
+    <t>—---—---</t>
+  </si>
+  <si>
+    <t>—---- -</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>*** Our Order Department is open until 6:30pm Eastern Time *#*</t>
+  </si>
+  <si>
+    <t>To pay this invoice when due, please follow Safilo's Remittance Instructions. If you need these</t>
+  </si>
+  <si>
+    <t>instructions, please email a request to AR.Inbox@safilo.com. Payment via eCheck is preferred. Safilo's</t>
+  </si>
+  <si>
+    <t>payment address is PO Box 35118, Newark, NJ 07193—5118 (please do not return merchandise to this address).</t>
+  </si>
+  <si>
+    <t>Thank you.</t>
+  </si>
+  <si>
+    <t>ORIGINAL INVOICE - PLEASE RETAIN FOR YOUR RECORDS 1050530</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A37"/>
+  <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -588,7 +588,7 @@
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1">
@@ -608,36 +608,31 @@
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>